<commit_message>
fix robot links' inertia
</commit_message>
<xml_diff>
--- a/hurba_robot_arm/urdf/inertia_calculator.xlsx
+++ b/hurba_robot_arm/urdf/inertia_calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\home\david\catkin_ws\src\Project-6-Robot-Arm\hurba_robot_arm\urdf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{604F0BCD-0AC7-4F64-BBE2-DFDE495A5DB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B5F8E5-D831-4AB5-A09D-4F13B8D28514}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{1B7231EA-3DDD-45D8-92DD-3817892A846F}"/>
+    <workbookView xWindow="6984" yWindow="2628" windowWidth="23040" windowHeight="12204" xr2:uid="{1B7231EA-3DDD-45D8-92DD-3817892A846F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -76,6 +76,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="170" formatCode="0.0000000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -111,8 +114,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,12 +434,13 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="5" max="7" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -573,19 +578,19 @@
         <v>0.1</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>4.6666648000000005E-2</v>
+        <v>9.333329600000001E-2</v>
       </c>
       <c r="F6">
         <f t="shared" si="1"/>
-        <v>4.6666648000000005E-2</v>
+        <v>9.333329600000001E-2</v>
       </c>
       <c r="G6">
         <f t="shared" si="2"/>
-        <v>1.0000000000000002E-2</v>
+        <v>2.0000000000000004E-2</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -599,19 +604,19 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="D7">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>4.2072899837499993E-3</v>
+        <v>8.4145799674999987E-3</v>
       </c>
       <c r="F7">
         <f t="shared" si="1"/>
-        <v>4.2072899837499993E-3</v>
+        <v>8.4145799674999987E-3</v>
       </c>
       <c r="G7">
         <f t="shared" si="2"/>
-        <v>1.4062499999999999E-3</v>
+        <v>2.8124999999999999E-3</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -625,19 +630,19 @@
         <v>0.1</v>
       </c>
       <c r="D8">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>8.1249967500000018E-4</v>
+        <v>2.7083322500000008E-4</v>
       </c>
       <c r="F8">
         <f t="shared" si="1"/>
-        <v>8.1249967500000018E-4</v>
+        <v>2.7083322500000008E-4</v>
       </c>
       <c r="G8">
         <f t="shared" si="2"/>
-        <v>1.5E-3</v>
+        <v>5.0000000000000012E-4</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -651,19 +656,19 @@
         <v>0.01</v>
       </c>
       <c r="D9">
-        <v>0.1</v>
-      </c>
-      <c r="E9">
+        <v>0.05</v>
+      </c>
+      <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>1.8999992400000002E-4</v>
-      </c>
-      <c r="F9">
+        <v>9.4999962000000008E-5</v>
+      </c>
+      <c r="F9" s="1">
         <f t="shared" si="1"/>
-        <v>1.8999992400000002E-4</v>
-      </c>
-      <c r="G9">
+        <v>9.4999962000000008E-5</v>
+      </c>
+      <c r="G9" s="1">
         <f t="shared" si="2"/>
-        <v>5.0000000000000004E-6</v>
+        <v>2.5000000000000002E-6</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -677,23 +682,24 @@
         <v>0.01</v>
       </c>
       <c r="D10">
-        <v>0.1</v>
-      </c>
-      <c r="E10">
+        <v>0.05</v>
+      </c>
+      <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>1.8999992400000002E-4</v>
-      </c>
-      <c r="F10">
+        <v>9.4999962000000008E-5</v>
+      </c>
+      <c r="F10" s="1">
         <f t="shared" si="1"/>
-        <v>1.8999992400000002E-4</v>
-      </c>
-      <c r="G10">
+        <v>9.4999962000000008E-5</v>
+      </c>
+      <c r="G10" s="1">
         <f t="shared" si="2"/>
-        <v>5.0000000000000004E-6</v>
+        <v>2.5000000000000002E-6</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>